<commit_message>
Correction of pressure level
- za + zp : low to medium
- mi: medium to high
- replaced NA w/ actual herm_cover values
</commit_message>
<xml_diff>
--- a/Multi-taxa_data/eDNA/2-Clean_data/Okinawa_ESV_taxon_table_NCsub_4excluded_2_85percent_threshold_metadata_rda.xlsx
+++ b/Multi-taxa_data/eDNA/2-Clean_data/Okinawa_ESV_taxon_table_NCsub_4excluded_2_85percent_threshold_metadata_rda.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8f76f43783816adf/Dokumente/PostDoc_Okinawa/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claud\Documents\COMUNE\STUDIO.LAVORO\IMBRSea\Thesis\StatAnalysis\Multi-taxa_data\eDNA\2-Clean_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C59D493-C598-40BA-9798-EA86873A51E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8160ACEB-CF41-4CB9-ADB1-A1AFED124AB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="95">
   <si>
     <t>Samples</t>
   </si>
@@ -103,39 +103,6 @@
     <t>Sukuta_shallow_seawater_1</t>
   </si>
   <si>
-    <t>Sakibaru2_shallow_seawater_3</t>
-  </si>
-  <si>
-    <t>Sakibaru2_shallow_seawater_1</t>
-  </si>
-  <si>
-    <t>Sakibaru2_deep_seawater_3</t>
-  </si>
-  <si>
-    <t>Sakibaru2_deep_seawater_2</t>
-  </si>
-  <si>
-    <t>Sakibaru2_deep_seawater_1</t>
-  </si>
-  <si>
-    <t>Sakibaru1_shallow_seawater_3</t>
-  </si>
-  <si>
-    <t>Sakibaru1_shallow_seawater_2</t>
-  </si>
-  <si>
-    <t>Sakibaru1_shallow_seawater_1</t>
-  </si>
-  <si>
-    <t>Sakibaru1_deep_seawater_3</t>
-  </si>
-  <si>
-    <t>Sakibaru1_deep_seawater_2</t>
-  </si>
-  <si>
-    <t>Sakibaru1_deep_seawater_1</t>
-  </si>
-  <si>
     <t>Mizugama_shallow_seawater_3</t>
   </si>
   <si>
@@ -241,12 +208,6 @@
     <t>Sukuta</t>
   </si>
   <si>
-    <t>Sakibaru2</t>
-  </si>
-  <si>
-    <t>Sakibaru1</t>
-  </si>
-  <si>
     <t>Mizugama</t>
   </si>
   <si>
@@ -304,10 +265,46 @@
     <t>herma_score</t>
   </si>
   <si>
-    <t>na</t>
-  </si>
-  <si>
     <t>other_pressures</t>
+  </si>
+  <si>
+    <t>Sakubaru2_shallow_seawater_3</t>
+  </si>
+  <si>
+    <t>Sakubaru2</t>
+  </si>
+  <si>
+    <t>Sakubaru2_shallow_seawater_1</t>
+  </si>
+  <si>
+    <t>Sakubaru2_deep_seawater_3</t>
+  </si>
+  <si>
+    <t>Sakubaru2_deep_seawater_2</t>
+  </si>
+  <si>
+    <t>Sakubaru2_deep_seawater_1</t>
+  </si>
+  <si>
+    <t>Sakubaru1_shallow_seawater_3</t>
+  </si>
+  <si>
+    <t>Sakubaru1</t>
+  </si>
+  <si>
+    <t>Sakubaru1_shallow_seawater_2</t>
+  </si>
+  <si>
+    <t>Sakubaru1_shallow_seawater_1</t>
+  </si>
+  <si>
+    <t>Sakubaru1_deep_seawater_3</t>
+  </si>
+  <si>
+    <t>Sakubaru1_deep_seawater_2</t>
+  </si>
+  <si>
+    <t>Sakubaru1_deep_seawater_1</t>
   </si>
 </sst>
 </file>
@@ -374,7 +371,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -387,10 +384,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -682,70 +675,70 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.109375" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D2" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="E2">
         <v>-1</v>
@@ -762,25 +755,25 @@
       <c r="I2">
         <v>0</v>
       </c>
-      <c r="J2" t="s">
-        <v>94</v>
+      <c r="J2">
+        <v>-0.5</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="E3">
         <v>-1</v>
@@ -797,25 +790,25 @@
       <c r="I3">
         <v>0</v>
       </c>
-      <c r="J3" t="s">
-        <v>94</v>
+      <c r="J3">
+        <v>-0.5</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D4" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="E4">
         <v>-1</v>
@@ -832,25 +825,25 @@
       <c r="I4">
         <v>0</v>
       </c>
-      <c r="J4" t="s">
-        <v>94</v>
+      <c r="J4">
+        <v>-0.5</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D5" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="E5">
         <v>-1</v>
@@ -867,25 +860,25 @@
       <c r="I5">
         <v>0</v>
       </c>
-      <c r="J5" t="s">
-        <v>94</v>
+      <c r="J5">
+        <v>-0.5</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C6" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D6" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="E6">
         <v>-1</v>
@@ -902,25 +895,25 @@
       <c r="I6">
         <v>0</v>
       </c>
-      <c r="J6" t="s">
-        <v>94</v>
+      <c r="J6">
+        <v>-0.5</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C7" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D7" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="E7">
         <v>-1</v>
@@ -937,25 +930,25 @@
       <c r="I7">
         <v>0</v>
       </c>
-      <c r="J7" t="s">
-        <v>94</v>
+      <c r="J7">
+        <v>-0.5</v>
       </c>
       <c r="K7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C8" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D8" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -979,18 +972,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C9" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D9" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1014,18 +1007,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D10" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1049,18 +1042,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C11" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D11" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -1084,18 +1077,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C12" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D12" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1119,18 +1112,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C13" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D13" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -1154,18 +1147,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C14" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D14" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1182,25 +1175,25 @@
       <c r="I14">
         <v>0</v>
       </c>
-      <c r="J14" t="s">
-        <v>94</v>
+      <c r="J14">
+        <v>-0.5</v>
       </c>
       <c r="K14">
         <v>-1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C15" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D15" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -1217,25 +1210,25 @@
       <c r="I15">
         <v>0</v>
       </c>
-      <c r="J15" t="s">
-        <v>94</v>
+      <c r="J15">
+        <v>-0.5</v>
       </c>
       <c r="K15">
         <v>-1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D16" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -1252,25 +1245,25 @@
       <c r="I16">
         <v>0</v>
       </c>
-      <c r="J16" t="s">
-        <v>94</v>
+      <c r="J16">
+        <v>-0.5</v>
       </c>
       <c r="K16">
         <v>-1</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C17" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D17" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -1287,25 +1280,25 @@
       <c r="I17">
         <v>0</v>
       </c>
-      <c r="J17" t="s">
-        <v>94</v>
+      <c r="J17">
+        <v>-0.5</v>
       </c>
       <c r="K17">
         <v>-1</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C18" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D18" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -1322,25 +1315,25 @@
       <c r="I18">
         <v>0</v>
       </c>
-      <c r="J18" t="s">
-        <v>94</v>
+      <c r="J18">
+        <v>-0.5</v>
       </c>
       <c r="K18">
         <v>-1</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C19" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D19" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E19">
         <v>-1</v>
@@ -1357,25 +1350,25 @@
       <c r="I19">
         <v>-1</v>
       </c>
-      <c r="J19" t="s">
-        <v>94</v>
+      <c r="J19">
+        <v>-1</v>
       </c>
       <c r="K19">
         <v>-1</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C20" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D20" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E20">
         <v>-1</v>
@@ -1399,18 +1392,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C21" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D21" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E21">
         <v>-1</v>
@@ -1434,18 +1427,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C22" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D22" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E22">
         <v>-1</v>
@@ -1469,18 +1462,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C23" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D23" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E23">
         <v>-1</v>
@@ -1504,18 +1497,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C24" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D24" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E24">
         <v>-1</v>
@@ -1539,18 +1532,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="C25" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D25" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="E25">
         <v>-1</v>
@@ -1567,25 +1560,25 @@
       <c r="I25">
         <v>-1</v>
       </c>
-      <c r="J25" t="s">
-        <v>94</v>
+      <c r="J25">
+        <v>-1</v>
       </c>
       <c r="K25">
         <v>-1</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="C26" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D26" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="E26">
         <v>-1</v>
@@ -1602,25 +1595,25 @@
       <c r="I26">
         <v>-1</v>
       </c>
-      <c r="J26" t="s">
-        <v>94</v>
+      <c r="J26">
+        <v>-1</v>
       </c>
       <c r="K26">
         <v>-1</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="C27" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D27" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="E27">
         <v>-1</v>
@@ -1637,830 +1630,830 @@
       <c r="I27">
         <v>-1</v>
       </c>
-      <c r="J27" t="s">
+      <c r="J27">
+        <v>-1</v>
+      </c>
+      <c r="K27">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" t="s">
+        <v>73</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>-0.5</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" t="s">
+        <v>73</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>-0.5</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" t="s">
+        <v>73</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>-0.5</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" t="s">
+        <v>73</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>-0.5</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>87</v>
+      </c>
+      <c r="B32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" t="s">
+        <v>73</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>-0.5</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>88</v>
+      </c>
+      <c r="B33" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33" t="s">
+        <v>73</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>-0.5</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>90</v>
+      </c>
+      <c r="B34" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" t="s">
+        <v>67</v>
+      </c>
+      <c r="D34" t="s">
+        <v>73</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>-0.5</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>91</v>
+      </c>
+      <c r="B35" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" t="s">
+        <v>67</v>
+      </c>
+      <c r="D35" t="s">
+        <v>73</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>-0.5</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>92</v>
+      </c>
+      <c r="B36" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" t="s">
+        <v>68</v>
+      </c>
+      <c r="D36" t="s">
+        <v>73</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>-0.5</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>93</v>
+      </c>
+      <c r="B37" t="s">
+        <v>89</v>
+      </c>
+      <c r="C37" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37" t="s">
+        <v>73</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <v>-0.5</v>
+      </c>
+      <c r="K37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>94</v>
       </c>
-      <c r="K27">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B38" t="s">
+        <v>89</v>
+      </c>
+      <c r="C38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D38" t="s">
+        <v>73</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <v>-0.5</v>
+      </c>
+      <c r="K38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>27</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B39" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39" t="s">
+        <v>67</v>
+      </c>
+      <c r="D39" t="s">
+        <v>72</v>
+      </c>
+      <c r="E39">
+        <v>-1</v>
+      </c>
+      <c r="F39">
+        <v>-1</v>
+      </c>
+      <c r="G39">
+        <v>-0.5</v>
+      </c>
+      <c r="H39">
+        <v>-0.5</v>
+      </c>
+      <c r="I39">
+        <v>-1</v>
+      </c>
+      <c r="J39">
+        <v>-1</v>
+      </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" t="s">
+        <v>72</v>
+      </c>
+      <c r="E40">
+        <v>-1</v>
+      </c>
+      <c r="F40">
+        <v>-1</v>
+      </c>
+      <c r="G40">
+        <v>-0.5</v>
+      </c>
+      <c r="H40">
+        <v>-0.5</v>
+      </c>
+      <c r="I40">
+        <v>-1</v>
+      </c>
+      <c r="J40">
+        <v>-1</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>29</v>
+      </c>
+      <c r="B41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" t="s">
+        <v>67</v>
+      </c>
+      <c r="D41" t="s">
+        <v>72</v>
+      </c>
+      <c r="E41">
+        <v>-1</v>
+      </c>
+      <c r="F41">
+        <v>-1</v>
+      </c>
+      <c r="G41">
+        <v>-0.5</v>
+      </c>
+      <c r="H41">
+        <v>-0.5</v>
+      </c>
+      <c r="I41">
+        <v>-1</v>
+      </c>
+      <c r="J41">
+        <v>-1</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42" t="s">
+        <v>68</v>
+      </c>
+      <c r="D42" t="s">
+        <v>72</v>
+      </c>
+      <c r="E42">
+        <v>-1</v>
+      </c>
+      <c r="F42">
+        <v>-1</v>
+      </c>
+      <c r="G42">
+        <v>-0.5</v>
+      </c>
+      <c r="H42">
+        <v>-0.5</v>
+      </c>
+      <c r="I42">
+        <v>-1</v>
+      </c>
+      <c r="J42">
+        <v>-1</v>
+      </c>
+      <c r="K42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" t="s">
+        <v>62</v>
+      </c>
+      <c r="C43" t="s">
+        <v>68</v>
+      </c>
+      <c r="D43" t="s">
+        <v>72</v>
+      </c>
+      <c r="E43">
+        <v>-1</v>
+      </c>
+      <c r="F43">
+        <v>-1</v>
+      </c>
+      <c r="G43">
+        <v>-0.5</v>
+      </c>
+      <c r="H43">
+        <v>-0.5</v>
+      </c>
+      <c r="I43">
+        <v>-1</v>
+      </c>
+      <c r="J43">
+        <v>-1</v>
+      </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44" t="s">
+        <v>68</v>
+      </c>
+      <c r="D44" t="s">
+        <v>72</v>
+      </c>
+      <c r="E44">
+        <v>-1</v>
+      </c>
+      <c r="F44">
+        <v>-1</v>
+      </c>
+      <c r="G44">
+        <v>-0.5</v>
+      </c>
+      <c r="H44">
+        <v>-0.5</v>
+      </c>
+      <c r="I44">
+        <v>-1</v>
+      </c>
+      <c r="J44">
+        <v>-1</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>33</v>
+      </c>
+      <c r="B45" t="s">
+        <v>63</v>
+      </c>
+      <c r="C45" t="s">
+        <v>67</v>
+      </c>
+      <c r="D45" t="s">
         <v>73</v>
       </c>
-      <c r="C28" t="s">
-        <v>80</v>
-      </c>
-      <c r="D28" t="s">
-        <v>86</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-      <c r="J28" t="s">
-        <v>94</v>
-      </c>
-      <c r="K28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>-0.5</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>34</v>
+      </c>
+      <c r="B46" t="s">
+        <v>63</v>
+      </c>
+      <c r="C46" t="s">
+        <v>67</v>
+      </c>
+      <c r="D46" t="s">
         <v>73</v>
       </c>
-      <c r="C29" t="s">
-        <v>80</v>
-      </c>
-      <c r="D29" t="s">
-        <v>86</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
-      <c r="I29">
-        <v>0</v>
-      </c>
-      <c r="J29" t="s">
-        <v>94</v>
-      </c>
-      <c r="K29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>-0.5</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>35</v>
+      </c>
+      <c r="B47" t="s">
+        <v>63</v>
+      </c>
+      <c r="C47" t="s">
+        <v>67</v>
+      </c>
+      <c r="D47" t="s">
         <v>73</v>
       </c>
-      <c r="C30" t="s">
-        <v>81</v>
-      </c>
-      <c r="D30" t="s">
-        <v>86</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="H30">
-        <v>0</v>
-      </c>
-      <c r="I30">
-        <v>0</v>
-      </c>
-      <c r="J30" t="s">
-        <v>94</v>
-      </c>
-      <c r="K30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31" t="s">
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>-0.5</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>36</v>
+      </c>
+      <c r="B48" t="s">
+        <v>63</v>
+      </c>
+      <c r="C48" t="s">
+        <v>68</v>
+      </c>
+      <c r="D48" t="s">
         <v>73</v>
       </c>
-      <c r="C31" t="s">
-        <v>81</v>
-      </c>
-      <c r="D31" t="s">
-        <v>86</v>
-      </c>
-      <c r="E31">
-        <v>0</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
-      <c r="H31">
-        <v>0</v>
-      </c>
-      <c r="I31">
-        <v>0</v>
-      </c>
-      <c r="J31" t="s">
-        <v>94</v>
-      </c>
-      <c r="K31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>31</v>
-      </c>
-      <c r="B32" t="s">
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>-0.5</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>37</v>
+      </c>
+      <c r="B49" t="s">
+        <v>63</v>
+      </c>
+      <c r="C49" t="s">
+        <v>68</v>
+      </c>
+      <c r="D49" t="s">
         <v>73</v>
       </c>
-      <c r="C32" t="s">
-        <v>81</v>
-      </c>
-      <c r="D32" t="s">
-        <v>86</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-      <c r="H32">
-        <v>0</v>
-      </c>
-      <c r="I32">
-        <v>0</v>
-      </c>
-      <c r="J32" t="s">
-        <v>94</v>
-      </c>
-      <c r="K32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33" t="s">
-        <v>74</v>
-      </c>
-      <c r="C33" t="s">
-        <v>80</v>
-      </c>
-      <c r="D33" t="s">
-        <v>86</v>
-      </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
-      <c r="H33">
-        <v>0</v>
-      </c>
-      <c r="I33">
-        <v>0</v>
-      </c>
-      <c r="J33" t="s">
-        <v>94</v>
-      </c>
-      <c r="K33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34" t="s">
-        <v>74</v>
-      </c>
-      <c r="C34" t="s">
-        <v>80</v>
-      </c>
-      <c r="D34" t="s">
-        <v>86</v>
-      </c>
-      <c r="E34">
-        <v>0</v>
-      </c>
-      <c r="F34">
-        <v>0</v>
-      </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-      <c r="H34">
-        <v>0</v>
-      </c>
-      <c r="I34">
-        <v>0</v>
-      </c>
-      <c r="J34" t="s">
-        <v>94</v>
-      </c>
-      <c r="K34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" t="s">
-        <v>74</v>
-      </c>
-      <c r="C35" t="s">
-        <v>80</v>
-      </c>
-      <c r="D35" t="s">
-        <v>86</v>
-      </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-      <c r="F35">
-        <v>0</v>
-      </c>
-      <c r="G35">
-        <v>0</v>
-      </c>
-      <c r="H35">
-        <v>0</v>
-      </c>
-      <c r="I35">
-        <v>0</v>
-      </c>
-      <c r="J35" t="s">
-        <v>94</v>
-      </c>
-      <c r="K35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>35</v>
-      </c>
-      <c r="B36" t="s">
-        <v>74</v>
-      </c>
-      <c r="C36" t="s">
-        <v>81</v>
-      </c>
-      <c r="D36" t="s">
-        <v>86</v>
-      </c>
-      <c r="E36">
-        <v>0</v>
-      </c>
-      <c r="F36">
-        <v>0</v>
-      </c>
-      <c r="G36">
-        <v>0</v>
-      </c>
-      <c r="H36">
-        <v>0</v>
-      </c>
-      <c r="I36">
-        <v>0</v>
-      </c>
-      <c r="J36" t="s">
-        <v>94</v>
-      </c>
-      <c r="K36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>36</v>
-      </c>
-      <c r="B37" t="s">
-        <v>74</v>
-      </c>
-      <c r="C37" t="s">
-        <v>81</v>
-      </c>
-      <c r="D37" t="s">
-        <v>86</v>
-      </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
-      <c r="F37">
-        <v>0</v>
-      </c>
-      <c r="G37">
-        <v>0</v>
-      </c>
-      <c r="H37">
-        <v>0</v>
-      </c>
-      <c r="I37">
-        <v>0</v>
-      </c>
-      <c r="J37" t="s">
-        <v>94</v>
-      </c>
-      <c r="K37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38" t="s">
-        <v>74</v>
-      </c>
-      <c r="C38" t="s">
-        <v>81</v>
-      </c>
-      <c r="D38" t="s">
-        <v>86</v>
-      </c>
-      <c r="E38">
-        <v>0</v>
-      </c>
-      <c r="F38">
-        <v>0</v>
-      </c>
-      <c r="G38">
-        <v>0</v>
-      </c>
-      <c r="H38">
-        <v>0</v>
-      </c>
-      <c r="I38">
-        <v>0</v>
-      </c>
-      <c r="J38" t="s">
-        <v>94</v>
-      </c>
-      <c r="K38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <v>-0.5</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>38</v>
       </c>
-      <c r="B39" t="s">
-        <v>75</v>
-      </c>
-      <c r="C39" t="s">
-        <v>80</v>
-      </c>
-      <c r="D39" t="s">
-        <v>87</v>
-      </c>
-      <c r="E39">
-        <v>-1</v>
-      </c>
-      <c r="F39">
-        <v>-1</v>
-      </c>
-      <c r="G39">
-        <v>-0.5</v>
-      </c>
-      <c r="H39">
-        <v>-0.5</v>
-      </c>
-      <c r="I39">
-        <v>-1</v>
-      </c>
-      <c r="J39" t="s">
-        <v>94</v>
-      </c>
-      <c r="K39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="B50" t="s">
+        <v>63</v>
+      </c>
+      <c r="C50" t="s">
+        <v>68</v>
+      </c>
+      <c r="D50" t="s">
+        <v>73</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>-0.5</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>39</v>
       </c>
-      <c r="B40" t="s">
-        <v>75</v>
-      </c>
-      <c r="C40" t="s">
-        <v>80</v>
-      </c>
-      <c r="D40" t="s">
-        <v>87</v>
-      </c>
-      <c r="E40">
-        <v>-1</v>
-      </c>
-      <c r="F40">
-        <v>-1</v>
-      </c>
-      <c r="G40">
-        <v>-0.5</v>
-      </c>
-      <c r="H40">
-        <v>-0.5</v>
-      </c>
-      <c r="I40">
-        <v>-1</v>
-      </c>
-      <c r="J40" t="s">
-        <v>94</v>
-      </c>
-      <c r="K40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>40</v>
-      </c>
-      <c r="B41" t="s">
-        <v>75</v>
-      </c>
-      <c r="C41" t="s">
-        <v>80</v>
-      </c>
-      <c r="D41" t="s">
-        <v>87</v>
-      </c>
-      <c r="E41">
-        <v>-1</v>
-      </c>
-      <c r="F41">
-        <v>-1</v>
-      </c>
-      <c r="G41">
-        <v>-0.5</v>
-      </c>
-      <c r="H41">
-        <v>-0.5</v>
-      </c>
-      <c r="I41">
-        <v>-1</v>
-      </c>
-      <c r="J41" t="s">
-        <v>94</v>
-      </c>
-      <c r="K41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>41</v>
-      </c>
-      <c r="B42" t="s">
-        <v>75</v>
-      </c>
-      <c r="C42" t="s">
-        <v>81</v>
-      </c>
-      <c r="D42" t="s">
-        <v>87</v>
-      </c>
-      <c r="E42">
-        <v>-1</v>
-      </c>
-      <c r="F42">
-        <v>-1</v>
-      </c>
-      <c r="G42">
-        <v>-0.5</v>
-      </c>
-      <c r="H42">
-        <v>-0.5</v>
-      </c>
-      <c r="I42">
-        <v>-1</v>
-      </c>
-      <c r="J42" t="s">
-        <v>94</v>
-      </c>
-      <c r="K42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>42</v>
-      </c>
-      <c r="B43" t="s">
-        <v>75</v>
-      </c>
-      <c r="C43" t="s">
-        <v>81</v>
-      </c>
-      <c r="D43" t="s">
-        <v>87</v>
-      </c>
-      <c r="E43">
-        <v>-1</v>
-      </c>
-      <c r="F43">
-        <v>-1</v>
-      </c>
-      <c r="G43">
-        <v>-0.5</v>
-      </c>
-      <c r="H43">
-        <v>-0.5</v>
-      </c>
-      <c r="I43">
-        <v>-1</v>
-      </c>
-      <c r="J43" t="s">
-        <v>94</v>
-      </c>
-      <c r="K43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>43</v>
-      </c>
-      <c r="B44" t="s">
-        <v>75</v>
-      </c>
-      <c r="C44" t="s">
-        <v>81</v>
-      </c>
-      <c r="D44" t="s">
-        <v>87</v>
-      </c>
-      <c r="E44">
-        <v>-1</v>
-      </c>
-      <c r="F44">
-        <v>-1</v>
-      </c>
-      <c r="G44">
-        <v>-0.5</v>
-      </c>
-      <c r="H44">
-        <v>-0.5</v>
-      </c>
-      <c r="I44">
-        <v>-1</v>
-      </c>
-      <c r="J44" t="s">
-        <v>94</v>
-      </c>
-      <c r="K44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>44</v>
-      </c>
-      <c r="B45" t="s">
-        <v>76</v>
-      </c>
-      <c r="C45" t="s">
-        <v>80</v>
-      </c>
-      <c r="D45" t="s">
-        <v>86</v>
-      </c>
-      <c r="E45">
-        <v>0</v>
-      </c>
-      <c r="F45">
-        <v>0</v>
-      </c>
-      <c r="G45">
-        <v>0</v>
-      </c>
-      <c r="H45">
-        <v>0</v>
-      </c>
-      <c r="I45">
-        <v>-0.5</v>
-      </c>
-      <c r="J45">
-        <v>0</v>
-      </c>
-      <c r="K45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>45</v>
-      </c>
-      <c r="B46" t="s">
-        <v>76</v>
-      </c>
-      <c r="C46" t="s">
-        <v>80</v>
-      </c>
-      <c r="D46" t="s">
-        <v>86</v>
-      </c>
-      <c r="E46">
-        <v>0</v>
-      </c>
-      <c r="F46">
-        <v>0</v>
-      </c>
-      <c r="G46">
-        <v>0</v>
-      </c>
-      <c r="H46">
-        <v>0</v>
-      </c>
-      <c r="I46">
-        <v>-0.5</v>
-      </c>
-      <c r="J46">
-        <v>0</v>
-      </c>
-      <c r="K46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>46</v>
-      </c>
-      <c r="B47" t="s">
-        <v>76</v>
-      </c>
-      <c r="C47" t="s">
-        <v>80</v>
-      </c>
-      <c r="D47" t="s">
-        <v>86</v>
-      </c>
-      <c r="E47">
-        <v>0</v>
-      </c>
-      <c r="F47">
-        <v>0</v>
-      </c>
-      <c r="G47">
-        <v>0</v>
-      </c>
-      <c r="H47">
-        <v>0</v>
-      </c>
-      <c r="I47">
-        <v>-0.5</v>
-      </c>
-      <c r="J47">
-        <v>0</v>
-      </c>
-      <c r="K47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>47</v>
-      </c>
-      <c r="B48" t="s">
-        <v>76</v>
-      </c>
-      <c r="C48" t="s">
-        <v>81</v>
-      </c>
-      <c r="D48" t="s">
-        <v>86</v>
-      </c>
-      <c r="E48">
-        <v>0</v>
-      </c>
-      <c r="F48">
-        <v>0</v>
-      </c>
-      <c r="G48">
-        <v>0</v>
-      </c>
-      <c r="H48">
-        <v>0</v>
-      </c>
-      <c r="I48">
-        <v>-0.5</v>
-      </c>
-      <c r="J48">
-        <v>0</v>
-      </c>
-      <c r="K48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>48</v>
-      </c>
-      <c r="B49" t="s">
-        <v>76</v>
-      </c>
-      <c r="C49" t="s">
-        <v>81</v>
-      </c>
-      <c r="D49" t="s">
-        <v>86</v>
-      </c>
-      <c r="E49">
-        <v>0</v>
-      </c>
-      <c r="F49">
-        <v>0</v>
-      </c>
-      <c r="G49">
-        <v>0</v>
-      </c>
-      <c r="H49">
-        <v>0</v>
-      </c>
-      <c r="I49">
-        <v>-0.5</v>
-      </c>
-      <c r="J49">
-        <v>0</v>
-      </c>
-      <c r="K49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>49</v>
-      </c>
-      <c r="B50" t="s">
-        <v>76</v>
-      </c>
-      <c r="C50" t="s">
-        <v>81</v>
-      </c>
-      <c r="D50" t="s">
-        <v>86</v>
-      </c>
-      <c r="E50">
-        <v>0</v>
-      </c>
-      <c r="F50">
-        <v>0</v>
-      </c>
-      <c r="G50">
-        <v>0</v>
-      </c>
-      <c r="H50">
-        <v>0</v>
-      </c>
-      <c r="I50">
-        <v>-0.5</v>
-      </c>
-      <c r="J50">
-        <v>0</v>
-      </c>
-      <c r="K50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>50</v>
-      </c>
       <c r="B51" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="C51" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D51" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E51">
         <v>-1</v>
@@ -2477,25 +2470,25 @@
       <c r="I51">
         <v>-1</v>
       </c>
-      <c r="J51" t="s">
-        <v>94</v>
+      <c r="J51">
+        <v>-1</v>
       </c>
       <c r="K51">
         <v>-1</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="B52" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="C52" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D52" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E52">
         <v>-1</v>
@@ -2512,25 +2505,25 @@
       <c r="I52">
         <v>-1</v>
       </c>
-      <c r="J52" t="s">
-        <v>94</v>
+      <c r="J52">
+        <v>-1</v>
       </c>
       <c r="K52">
         <v>-1</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B53" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="C53" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D53" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E53">
         <v>-1</v>
@@ -2547,25 +2540,25 @@
       <c r="I53">
         <v>-1</v>
       </c>
-      <c r="J53" t="s">
-        <v>94</v>
+      <c r="J53">
+        <v>-1</v>
       </c>
       <c r="K53">
         <v>-1</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B54" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="C54" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D54" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E54">
         <v>-1</v>
@@ -2582,25 +2575,25 @@
       <c r="I54">
         <v>-1</v>
       </c>
-      <c r="J54" t="s">
-        <v>94</v>
+      <c r="J54">
+        <v>-1</v>
       </c>
       <c r="K54">
         <v>-1</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B55" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="C55" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D55" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E55">
         <v>-1</v>
@@ -2617,25 +2610,25 @@
       <c r="I55">
         <v>-1</v>
       </c>
-      <c r="J55" t="s">
-        <v>94</v>
+      <c r="J55">
+        <v>-1</v>
       </c>
       <c r="K55">
         <v>-1</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B56" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="C56" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D56" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E56">
         <v>-1</v>
@@ -2652,25 +2645,25 @@
       <c r="I56">
         <v>-1</v>
       </c>
-      <c r="J56" t="s">
-        <v>94</v>
+      <c r="J56">
+        <v>-1</v>
       </c>
       <c r="K56">
         <v>-1</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="B57" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="C57" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D57" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E57">
         <v>-1</v>
@@ -2687,25 +2680,25 @@
       <c r="I57">
         <v>-1</v>
       </c>
-      <c r="J57" t="s">
-        <v>94</v>
+      <c r="J57">
+        <v>-1</v>
       </c>
       <c r="K57">
         <v>-1</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B58" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="C58" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D58" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E58">
         <v>-1</v>
@@ -2722,25 +2715,25 @@
       <c r="I58">
         <v>-1</v>
       </c>
-      <c r="J58" t="s">
-        <v>94</v>
+      <c r="J58">
+        <v>-1</v>
       </c>
       <c r="K58">
         <v>-1</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B59" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="C59" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D59" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E59">
         <v>-1</v>
@@ -2757,25 +2750,25 @@
       <c r="I59">
         <v>-1</v>
       </c>
-      <c r="J59" t="s">
-        <v>94</v>
+      <c r="J59">
+        <v>-1</v>
       </c>
       <c r="K59">
         <v>-1</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B60" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="C60" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D60" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E60">
         <v>-1</v>
@@ -2792,25 +2785,25 @@
       <c r="I60">
         <v>-1</v>
       </c>
-      <c r="J60" t="s">
-        <v>94</v>
+      <c r="J60">
+        <v>-1</v>
       </c>
       <c r="K60">
         <v>-1</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B61" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="C61" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D61" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E61">
         <v>-1</v>
@@ -2827,25 +2820,25 @@
       <c r="I61">
         <v>-1</v>
       </c>
-      <c r="J61" t="s">
-        <v>94</v>
+      <c r="J61">
+        <v>-1</v>
       </c>
       <c r="K61">
         <v>-1</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="B62" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="C62" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D62" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E62">
         <v>-1</v>
@@ -2862,25 +2855,25 @@
       <c r="I62">
         <v>-1</v>
       </c>
-      <c r="J62" t="s">
-        <v>94</v>
+      <c r="J62">
+        <v>-1</v>
       </c>
       <c r="K62">
         <v>-1</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B63" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="C63" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D63" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E63">
         <v>-1</v>
@@ -2904,18 +2897,18 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B64" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="C64" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D64" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E64">
         <v>-1</v>
@@ -2939,18 +2932,18 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B65" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="C65" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D65" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E65">
         <v>-1</v>
@@ -2974,18 +2967,18 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B66" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="C66" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D66" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E66">
         <v>-1</v>
@@ -3009,18 +3002,18 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
+        <v>55</v>
+      </c>
+      <c r="B67" t="s">
         <v>66</v>
       </c>
-      <c r="B67" t="s">
-        <v>79</v>
-      </c>
       <c r="C67" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D67" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E67">
         <v>-1</v>
@@ -3044,18 +3037,18 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B68" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="C68" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D68" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E68">
         <v>-1</v>

</xml_diff>